<commit_message>
update data and report
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pozzi\Documents\Projects\pizza_chart\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63844047-D0C9-47B6-B19C-6CF7CB2691E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CC4411-F645-4B6F-8D8F-108DDD021EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -134,9 +134,6 @@
   </si>
   <si>
     <t>Salame piccante</t>
-  </si>
-  <si>
-    <t>Parmigiana senza zola</t>
   </si>
   <si>
     <t>Wurstel e patatine</t>
@@ -334,6 +331,9 @@
   </si>
   <si>
     <t>Salsiccia e bufala</t>
+  </si>
+  <si>
+    <t>Parmigiana</t>
   </si>
 </sst>
 </file>
@@ -538,6 +538,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -552,7 +553,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -634,8 +634,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Orders" displayName="Orders" ref="A1:D37">
-  <autoFilter ref="A1:D37" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Orders" displayName="Orders" ref="A1:D43">
+  <autoFilter ref="A1:D43" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Pizza"/>
@@ -874,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -928,12 +928,12 @@
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
@@ -948,10 +948,10 @@
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="19"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
@@ -966,10 +966,10 @@
       <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="19"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
@@ -984,17 +984,17 @@
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>45603</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -1002,17 +1002,17 @@
       <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="19"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
         <v>45603</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -1020,17 +1020,17 @@
       <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="22"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="23"/>
     </row>
     <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
         <v>45603</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -1044,7 +1044,7 @@
         <v>45603</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -1058,13 +1058,13 @@
         <v>45610</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1078,7 +1078,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1086,13 +1086,13 @@
         <v>45610</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2">
         <v>4</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1100,13 +1100,13 @@
         <v>45610</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1114,13 +1114,13 @@
         <v>45610</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1134,7 +1134,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1148,7 +1148,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1156,13 +1156,13 @@
         <v>45610</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="2">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1170,13 +1170,13 @@
         <v>45617</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" s="2">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1190,7 +1190,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1198,13 +1198,13 @@
         <v>45617</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1212,13 +1212,13 @@
         <v>45617</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C22" s="2">
         <v>4</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1232,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1240,13 +1240,13 @@
         <v>45644</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24" s="2">
         <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1254,13 +1254,13 @@
         <v>45644</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="2">
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1274,7 +1274,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1282,13 +1282,13 @@
         <v>45674</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="2">
         <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1296,13 +1296,13 @@
         <v>45674</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28" s="2">
         <v>2</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1310,13 +1310,13 @@
         <v>45674</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C29" s="2">
         <v>4</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1330,7 +1330,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1344,7 +1344,7 @@
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1352,13 +1352,13 @@
         <v>45674</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32" s="2">
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -1366,31 +1366,31 @@
         <v>45680</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C33" s="2">
         <v>4</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="24">
+      <c r="A34" s="14">
         <v>45687</v>
       </c>
       <c r="B34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C34" s="2">
         <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="24">
+      <c r="A35" s="14">
         <v>45687</v>
       </c>
       <c r="B35" t="s">
@@ -1400,11 +1400,11 @@
         <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="24">
+      <c r="A36" s="14">
         <v>45687</v>
       </c>
       <c r="B36" t="s">
@@ -1414,40 +1414,106 @@
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="24">
+      <c r="A37" s="14">
         <v>45687</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C37" s="2">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C38" s="2"/>
+      <c r="A38" s="14">
+        <v>45695</v>
+      </c>
+      <c r="B38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="2">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="39" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C39" s="2"/>
+      <c r="A39" s="14">
+        <v>45695</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="2">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="40" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C40" s="2"/>
+      <c r="A40" s="14">
+        <v>45695</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="2">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="41" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C41" s="2"/>
+      <c r="A41" s="14">
+        <v>45695</v>
+      </c>
+      <c r="B41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="42" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C42" s="2"/>
+      <c r="A42" s="14">
+        <v>45695</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="2">
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="43" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C43" s="2"/>
+      <c r="A43" s="14">
+        <v>45695</v>
+      </c>
+      <c r="B43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="44" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C44" s="2"/>
@@ -4348,12 +4414,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="19.1328125" customWidth="1"/>
     <col min="3" max="3" width="13.1328125" customWidth="1"/>
     <col min="4" max="12" width="11.53125" customWidth="1"/>
@@ -4370,37 +4437,37 @@
         <v>2</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -4417,19 +4484,19 @@
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
@@ -4463,13 +4530,13 @@
       </c>
       <c r="C3" s="6">
         <f>IF(SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#])=0,"",SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#]))</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -4484,12 +4551,12 @@
         <v>45603</v>
       </c>
       <c r="O3" s="5"/>
-      <c r="P3" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="16"/>
+      <c r="P3" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="17"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
@@ -4511,19 +4578,19 @@
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -4535,10 +4602,10 @@
         <v>45603</v>
       </c>
       <c r="O4" s="5"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="19"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="20"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
@@ -4560,16 +4627,16 @@
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -4582,10 +4649,10 @@
         <v>45603</v>
       </c>
       <c r="O5" s="5"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="19"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="20"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
@@ -4604,13 +4671,13 @@
       </c>
       <c r="C6" s="6">
         <f>IF(SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#])=0,"",SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#]))</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>10</v>
@@ -4627,10 +4694,10 @@
         <v>45603</v>
       </c>
       <c r="O6" s="5"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="19"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="20"/>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
@@ -4641,30 +4708,27 @@
     </row>
     <row r="7" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" t="str">
-        <v>Parmigiana senza zola</v>
+        <v>Parmigiana</v>
       </c>
       <c r="B7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>Parmigiana senza zola</v>
+        <v>Parmigiana</v>
       </c>
       <c r="C7" s="6">
         <f>IF(SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#])=0,"",SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#]))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>48</v>
+        <v>40</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -4676,10 +4740,10 @@
         <v>45603</v>
       </c>
       <c r="O7" s="5"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="22"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
+      <c r="S7" s="23"/>
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
@@ -4698,19 +4762,19 @@
       </c>
       <c r="C8" s="6">
         <f>IF(SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#])=0,"",SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#]))</f>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -4748,16 +4812,16 @@
         <v>1</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>51</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -4795,13 +4859,13 @@
         <v>1</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -4840,16 +4904,16 @@
         <v>1</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>53</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>54</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -4887,13 +4951,13 @@
         <v>1</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -4929,19 +4993,19 @@
       </c>
       <c r="C13" s="6">
         <f>IF(SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#])=0,"",SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#]))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
@@ -4979,19 +5043,19 @@
         <v>2</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="H14" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -5028,22 +5092,22 @@
         <v>3</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -5079,13 +5143,13 @@
         <v>1</v>
       </c>
       <c r="D16" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -5124,13 +5188,13 @@
         <v>2</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
@@ -5157,19 +5221,19 @@
         <v>1</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
@@ -5191,16 +5255,16 @@
       </c>
       <c r="C19" s="6">
         <f>IF(SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#])=0,"",SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#]))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>54</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>

</xml_diff>

<commit_message>
fix last order data and update charts
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pozzi\Documents\Projects\pizza_chart\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B19183-F288-4F69-B65B-DFC3F6888DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE28132C-2659-4C35-95FF-CB93A7DA8F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -694,8 +694,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Orders" displayName="Orders" ref="A1:D59">
-  <autoFilter ref="A1:D59" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Orders" displayName="Orders" ref="A1:D60">
+  <autoFilter ref="A1:D60" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Pizza"/>
@@ -948,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1814,7 +1814,18 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C60" s="2"/>
+      <c r="A60" s="14">
+        <v>45723</v>
+      </c>
+      <c r="B60" t="s">
+        <v>57</v>
+      </c>
+      <c r="C60" s="2">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="61" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C61" s="2"/>
@@ -4966,7 +4977,7 @@
       </c>
       <c r="C7" s="6">
         <f>IF(SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#])=0,"",SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#]))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>35</v>
@@ -7988,7 +7999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update data and pizzas
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pozzi\Documents\Projects\pizza_chart\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A8A1E0-D65C-40F5-AF4B-E48BBE6CC89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F3DBFE-B5F6-4EEE-AB6D-3F562ABBA07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="69">
   <si>
     <t>Date</t>
   </si>
@@ -366,7 +366,19 @@
     <t>Crocken</t>
   </si>
   <si>
-    <t xml:space="preserve">Prosciutto </t>
+    <t>Crudo e grana</t>
+  </si>
+  <si>
+    <t>Speciale bianca</t>
+  </si>
+  <si>
+    <t>Prosciutto cotto</t>
+  </si>
+  <si>
+    <t>Prosciutto crudo</t>
+  </si>
+  <si>
+    <t>Wurstel</t>
   </si>
 </sst>
 </file>
@@ -559,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -616,6 +628,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -720,8 +735,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Orders" displayName="Orders" ref="A1:D75">
-  <autoFilter ref="A1:D75" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Orders" displayName="Orders" ref="A1:D79">
+  <autoFilter ref="A1:D79" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Pizza"/>
@@ -974,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2064,16 +2079,60 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C76" s="2"/>
+      <c r="A76" s="14">
+        <v>45804</v>
+      </c>
+      <c r="B76" t="s">
+        <v>64</v>
+      </c>
+      <c r="C76" s="2">
+        <v>1</v>
+      </c>
+      <c r="D76" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="77" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C77" s="2"/>
+      <c r="A77" s="14">
+        <v>45804</v>
+      </c>
+      <c r="B77" t="s">
+        <v>65</v>
+      </c>
+      <c r="C77" s="2">
+        <v>1</v>
+      </c>
+      <c r="D77" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="78" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C78" s="2"/>
+      <c r="A78" s="14">
+        <v>45804</v>
+      </c>
+      <c r="B78" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78" s="2">
+        <v>1</v>
+      </c>
+      <c r="D78" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="79" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C79" s="2"/>
+      <c r="A79" s="14">
+        <v>45804</v>
+      </c>
+      <c r="B79" t="s">
+        <v>16</v>
+      </c>
+      <c r="C79" s="2">
+        <v>1</v>
+      </c>
+      <c r="D79" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="80" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C80" s="2"/>
@@ -4887,8 +4946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4945,7 +5004,7 @@
     </row>
     <row r="2" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="str" cm="1">
-        <f t="array" ref="A2:A22">_xlfn.UNIQUE(Orders[Pizza])</f>
+        <f t="array" ref="A2:A24">_xlfn.UNIQUE(Orders[Pizza])</f>
         <v>Siciliana</v>
       </c>
       <c r="B2" s="5" t="str">
@@ -5282,7 +5341,7 @@
       </c>
       <c r="C9" s="6">
         <f>IF(SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#])=0,"",SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#]))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>34</v>
@@ -5466,7 +5525,7 @@
       </c>
       <c r="C13" s="6">
         <f>IF(SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#])=0,"",SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#]))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>34</v>
@@ -5474,8 +5533,8 @@
       <c r="E13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="13" t="s">
-        <v>21</v>
+      <c r="F13" s="18" t="s">
+        <v>66</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>45</v>
@@ -5521,8 +5580,8 @@
       <c r="E14" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="13" t="s">
-        <v>21</v>
+      <c r="F14" s="18" t="s">
+        <v>66</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>36</v>
@@ -5618,7 +5677,7 @@
         <v>39</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -5840,8 +5899,8 @@
       <c r="F22" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G22" s="19" t="s">
-        <v>64</v>
+      <c r="G22" s="30" t="s">
+        <v>66</v>
       </c>
       <c r="H22" s="19" t="s">
         <v>48</v>
@@ -5856,51 +5915,75 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="16" t="str">
+        <v>Crudo e grana</v>
+      </c>
       <c r="B23" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C23" s="6" t="str">
+        <v>Crudo e grana</v>
+      </c>
+      <c r="C23" s="6">
         <f>IF(SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#])=0,"",SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#]))</f>
-        <v/>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
-      <c r="N23" s="8" t="str">
+      <c r="N23" s="8">
         <f>IF(_xlfn.MINIFS(Orders[Date],Orders[Pizza],Pizza[[#This Row],[Pizza]])=0,"",_xlfn.MINIFS(Orders[Date],Orders[Pizza],Pizza[[#This Row],[Pizza]]))</f>
-        <v/>
+        <v>45804</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="16" t="str">
+        <v>Speciale bianca</v>
+      </c>
       <c r="B24" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C24" s="6" t="str">
+        <v>Speciale bianca</v>
+      </c>
+      <c r="C24" s="6">
         <f>IF(SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#])=0,"",SUMIF(Orders[Pizza],Pizza[[#This Row],[Pizza]],Orders['#]))</f>
-        <v/>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
-      <c r="N24" s="8" t="str">
+      <c r="N24" s="8">
         <f>IF(_xlfn.MINIFS(Orders[Date],Orders[Pizza],Pizza[[#This Row],[Pizza]])=0,"",_xlfn.MINIFS(Orders[Date],Orders[Pizza],Pizza[[#This Row],[Pizza]]))</f>
-        <v/>
+        <v>45804</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -8251,11 +8334,11 @@
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A29">_xlfn.UNIQUE(_xlfn.TOCOL(Pizza[[Topping 1]:[Topping 10]]))</f>
+        <f t="array" ref="A2:A30">_xlfn.UNIQUE(_xlfn.TOCOL(Pizza[[Topping 1]:[Topping 10]]))</f>
         <v>Pomodoro</v>
       </c>
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:B28">_xlfn._xlws.FILTER(A:A,A:A&lt;&gt;0)</f>
+        <f t="array" ref="B2:B29">_xlfn._xlws.FILTER(A:A,A:A&lt;&gt;0)</f>
         <v>Pomodoro</v>
       </c>
       <c r="C2" t="str">
@@ -8496,16 +8579,16 @@
         <v>Salsiccia</v>
       </c>
       <c r="B22" t="str">
-        <v>Prosciutto</v>
+        <v>Prosciutto cotto</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
-        <v>Prosciutto</v>
+        <v>Prosciutto cotto</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" t="str">
-        <v>Prosciutto</v>
+        <v>Prosciutto cotto</v>
       </c>
       <c r="B23" t="str">
         <v>Carciofini</v>
@@ -8568,23 +8651,29 @@
         <v>Peperoni</v>
       </c>
       <c r="B28" t="str">
-        <v xml:space="preserve">Prosciutto </v>
+        <v>Prosciutto crudo</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Prosciutto </v>
+        <v>Prosciutto crudo</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" t="str">
-        <v xml:space="preserve">Prosciutto </v>
+        <v>Prosciutto crudo</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Wurstel</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Wurstel</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" t="str">
+        <v>Wurstel</v>
+      </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
         <v/>

</xml_diff>

<commit_message>
move scripts to scripts folder
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pozzi\Documents\Projects\pizza_chart\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41F3DBFE-B5F6-4EEE-AB6D-3F562ABBA07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B18E95-C15C-4A89-A408-BBF76EC9A3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -616,6 +616,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -628,9 +631,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -989,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1007"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1043,12 +1043,12 @@
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="23"/>
     </row>
     <row r="4" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
@@ -1063,10 +1063,10 @@
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="26"/>
     </row>
     <row r="5" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
@@ -1081,10 +1081,10 @@
       <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="25"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="26"/>
     </row>
     <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
@@ -1099,10 +1099,10 @@
       <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="25"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="26"/>
     </row>
     <row r="7" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
@@ -1117,10 +1117,10 @@
       <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="25"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="26"/>
     </row>
     <row r="8" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
@@ -1135,10 +1135,10 @@
       <c r="D8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="28"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="29"/>
     </row>
     <row r="9" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3">
@@ -4946,8 +4946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -5083,12 +5083,12 @@
         <v>45603</v>
       </c>
       <c r="O3" s="5"/>
-      <c r="P3" s="29" t="s">
+      <c r="P3" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="23"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
@@ -5134,10 +5134,10 @@
         <v>45603</v>
       </c>
       <c r="O4" s="5"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="25"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="26"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
@@ -5181,10 +5181,10 @@
         <v>45603</v>
       </c>
       <c r="O5" s="5"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="24"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="25"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="26"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
@@ -5226,10 +5226,10 @@
         <v>45603</v>
       </c>
       <c r="O6" s="5"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="24"/>
-      <c r="S6" s="25"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="26"/>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
@@ -5272,10 +5272,10 @@
         <v>45603</v>
       </c>
       <c r="O7" s="5"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="28"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="29"/>
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
@@ -5899,7 +5899,7 @@
       <c r="F22" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G22" s="20" t="s">
         <v>66</v>
       </c>
       <c r="H22" s="19" t="s">

</xml_diff>

<commit_message>
update content on manual workflow trigger
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pozzi\Documents\Projects\pizza_chart\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B18E95-C15C-4A89-A408-BBF76EC9A3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EECBB70-764F-49FD-BBE0-D72DA70F48D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -989,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1007"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4946,8 +4946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -8307,7 +8307,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Append data from CSV
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -708,7 +708,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1014"/>
+  <dimension ref="A1:I1021"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
@@ -5057,9 +5057,6 @@
           <t xml:space="preserve"> 1 Da Rida</t>
         </is>
       </c>
-      <c r="D1012" t="n">
-        <v/>
-      </c>
     </row>
     <row r="1013">
       <c r="A1013" t="inlineStr">
@@ -5100,6 +5097,146 @@
         </is>
       </c>
       <c r="D1014" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Da Rida</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>17/06/2025</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Tonno e cipolle</t>
+        </is>
+      </c>
+      <c r="C1015" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1015" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Da Rida</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>17/06/2025</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Prosciutto e funghi bianca</t>
+        </is>
+      </c>
+      <c r="C1016" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1016" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Da Rida</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>17/06/2025</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Margherita</t>
+        </is>
+      </c>
+      <c r="C1017" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1017" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Da Rida</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>17/06/2025</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Tonno e peperoni</t>
+        </is>
+      </c>
+      <c r="C1018" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1018" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Da Rida</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>17/06/2025</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Speciale bianca</t>
+        </is>
+      </c>
+      <c r="C1019" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1019" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Da Rida</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>17/06/2025</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Crudo e bufala</t>
+        </is>
+      </c>
+      <c r="C1020" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1020" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Da Rida</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>17/06/2025</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Salame piccante</t>
+        </is>
+      </c>
+      <c r="C1021" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1021" t="inlineStr">
         <is>
           <t xml:space="preserve"> Da Rida</t>
         </is>

</xml_diff>